<commit_message>
Activate NO2 and RG
</commit_message>
<xml_diff>
--- a/inst/extdata/dist_df.xlsx
+++ b/inst/extdata/dist_df.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stani/GitHub/distreg.vis/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15D7B65-74C1-F341-88CF-612822EAE817}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB80C908-4505-1A4F-8BCD-94584B43D15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2684,10 +2684,10 @@
         <v>9</v>
       </c>
       <c r="C54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -2892,10 +2892,10 @@
         <v>9</v>
       </c>
       <c r="C62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Fix multinomial family and problems with non-existent moments
</commit_message>
<xml_diff>
--- a/inst/extdata/dist_df.xlsx
+++ b/inst/extdata/dist_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stani/GitHub/distreg.vis/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB80C908-4505-1A4F-8BCD-94584B43D15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AAA468-ADE8-8E4F-9A29-4102E9A8664F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4195,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E112">
         <v>0</v>
@@ -4426,7 +4426,7 @@
         <v>123</v>
       </c>
       <c r="C121" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D121" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
Change poisson limit and make limits in Excel numeric
</commit_message>
<xml_diff>
--- a/inst/extdata/dist_df.xlsx
+++ b/inst/extdata/dist_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stani/GitHub/distreg.vis/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AAA468-ADE8-8E4F-9A29-4102E9A8664F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AA052B-D08A-2F4E-B276-6982E220A216}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="142">
   <si>
     <t>dist_name</t>
   </si>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4483,8 +4483,8 @@
       <c r="D123" t="s">
         <v>56</v>
       </c>
-      <c r="E123" t="s">
-        <v>13</v>
+      <c r="E123">
+        <v>0</v>
       </c>
       <c r="F123" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Some error with implemented column
</commit_message>
<xml_diff>
--- a/inst/extdata/dist_df.xlsx
+++ b/inst/extdata/dist_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stani/GitHub/distreg.vis/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCAB957-4B73-9B4A-B37F-297F63F8101C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23ECCA1-0183-1746-B638-FD653D379C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1944,7 +1944,7 @@
       <c r="B41" t="s">
         <v>9</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="b">
         <v>1</v>
       </c>
       <c r="D41" t="s">

</xml_diff>